<commit_message>
Implement login management in TikTok Search Tool, enhancing user experience with automatic login prompts and session persistence. Updated configuration messages for login status and added functionality to save search results with user authentication. Removed example usage script to streamline the project structure.
</commit_message>
<xml_diff>
--- a/tiktok_search_cat.xlsx
+++ b/tiktok_search_cat.xlsx
@@ -512,22 +512,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/@theparsnipdiaries/video/7544092493378342166</t>
+          <t>https://www.tiktok.com/@wildmane_mainecoons/video/7544160476519779615</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>theparsnipdiaries</t>
+          <t>wildmane_mainecoons</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7544092493378342166</t>
+          <t>7544160476519779615</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Video by @theparsnipdiaries</t>
+          <t>Video by @wildmane_mainecoons</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -539,22 +539,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/@wildmane_mainecoons/video/7544160476519779615</t>
+          <t>https://www.tiktok.com/@cute.catsxxx/video/7543767375758265655</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>wildmane_mainecoons</t>
+          <t>cute.catsxxx</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>7544160476519779615</t>
+          <t>7543767375758265655</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Video by @wildmane_mainecoons</t>
+          <t>Video by @cute.catsxxx</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -566,22 +566,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/@funnypets.oftiktok/video/7543779397891820831</t>
+          <t>https://www.tiktok.com/@catutucom/video/7543337508155804935</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>funnypets.oftiktok</t>
+          <t>catutucom</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>7543779397891820831</t>
+          <t>7543337508155804935</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Video by @funnypets.oftiktok</t>
+          <t>Video by @catutucom</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -593,22 +593,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/@jfxgw/video/7542936311838100791</t>
+          <t>https://www.tiktok.com/@icecreamtina0/video/7543814939123666196</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>jfxgw</t>
+          <t>icecreamtina0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>7542936311838100791</t>
+          <t>7543814939123666196</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Video by @jfxgw</t>
+          <t>Video by @icecreamtina0</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">

</xml_diff>